<commit_message>
update import product from xlsx
</commit_message>
<xml_diff>
--- a/public/backend/file/product_import_list.xlsx
+++ b/public/backend/file/product_import_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luanp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Đường kính</t>
   </si>
@@ -53,28 +53,52 @@
     <t>Cái</t>
   </si>
   <si>
-    <t>có</t>
-  </si>
-  <si>
     <t>Tên hàng</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>Premium</t>
+    <t>không</t>
+  </si>
+  <si>
+    <t>B06-10.6-Standard Isee B&amp;L</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Thương hiệu</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Isee B&amp;L</t>
+  </si>
+  <si>
+    <t>Standard Isee B&amp;L</t>
+  </si>
+  <si>
+    <t>B05-10.6-Standard</t>
+  </si>
+  <si>
+    <t>Fargo</t>
+  </si>
+  <si>
+    <t>Dung dịch thử nghiệm</t>
   </si>
   <si>
     <t>Dung dịch</t>
   </si>
   <si>
-    <t>chai</t>
-  </si>
-  <si>
-    <t>không</t>
-  </si>
-  <si>
-    <t>Dung dịch thử nghiệm</t>
+    <t>Chai</t>
   </si>
 </sst>
 </file>
@@ -123,9 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,89 +432,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="2"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>10.5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>4.75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>